<commit_message>
Update Sprint Backlog to Add Users
Adjusted Sprint backlog to include officer capabilities to add new users, assigned to Ezra
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog.xlsx
+++ b/documentation/Sprint Backlog.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rs00207\Documents\GitHub\PirateShipInventoryManagementSystem\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9213A0E-386A-4EDD-80D9-777E9FB5483E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF956A0-A361-4D4A-AB8E-0CD4D7EE7091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="1755" windowWidth="21765" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3045" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>Related User Story</t>
   </si>
@@ -127,6 +136,12 @@
   </si>
   <si>
     <t>Nick</t>
+  </si>
+  <si>
+    <t>Manage User Accounts And Roles</t>
+  </si>
+  <si>
+    <t>Implement Officer's Adding New Users</t>
   </si>
 </sst>
 </file>
@@ -222,13 +237,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
@@ -344,7 +359,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -496,7 +511,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -504,6 +518,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1401,38 +1416,38 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
     <col min="2" max="2" width="59.140625" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1445,7 +1460,7 @@
       <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1601,14 +1616,14 @@
         <v>16</v>
       </c>
       <c r="C11" s="1">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1673,14 +1688,14 @@
         <v>25</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1701,16 +1716,25 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1719,7 +1743,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1728,7 +1752,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1737,7 +1761,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1746,7 +1770,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1755,7 +1779,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1764,7 +1788,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1773,7 +1797,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1782,7 +1806,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1791,13 +1815,13 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="3">
         <f>SUM(C3:C26)</f>
-        <v>20</v>
+        <v>20.5</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" ref="D27:G27" si="0">SUM(D3:D26)</f>

</xml_diff>

<commit_message>
Create ViewInventoryPage .fxml, CodeBehind, and ViewModel
Created the view inventory page's fxml, codebehind, and viewmodel. Added Jacoco to pom file to test code coverage. Created TestViewInventoryPageViewModel and recievd 100% code coverage for added implementation. Updated sprint backlog amount of time remaining on task for Monday and Tuesday.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog.xlsx
+++ b/documentation/Sprint Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rs00207\Documents\GitHub\PirateShipInventoryManagementSystem\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3CC5DC-FC65-47B5-A1C5-BA473F30C447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA1ACED-C34D-4B91-AF8D-C61E520EA3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="1755" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2310" yWindow="1785" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -359,7 +359,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1412,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,7 +1475,9 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1493,7 +1495,9 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1511,7 +1515,9 @@
       <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1529,7 +1535,9 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1547,7 +1555,9 @@
       <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1565,7 +1575,9 @@
       <c r="C8" s="1">
         <v>3</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1583,7 +1595,9 @@
       <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1601,7 +1615,9 @@
       <c r="C10" s="1">
         <v>1.5</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>1.5</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1619,7 +1635,9 @@
       <c r="C11" s="1">
         <v>0.5</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1637,7 +1655,9 @@
       <c r="C12" s="1">
         <v>1.5</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1655,7 +1675,9 @@
       <c r="C13" s="1">
         <v>0.5</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1673,7 +1695,9 @@
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1691,7 +1715,9 @@
       <c r="C15" s="1">
         <v>0.5</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1709,7 +1735,9 @@
       <c r="C16" s="1">
         <v>2</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1727,7 +1755,9 @@
       <c r="C17" s="1">
         <v>1.5</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1826,7 +1856,7 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" ref="D27:G27" si="0">SUM(D3:D26)</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Implement View Inventory Filters with Cook User Role
Added filtering for the view inventory page for Cook user role. Added Cook user within authenticator, Added checkIfCook method within landing page view model, Added permission for cooks to access view inventory page. Added Tests for all implemented additions. Updated sprint backlog for feature's task remaining hours.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog.xlsx
+++ b/documentation/Sprint Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rs00207\Documents\GitHub\PirateShipInventoryManagementSystem\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA1ACED-C34D-4B91-AF8D-C61E520EA3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DEA193-E697-44BB-823A-8BBE82F51EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2310" yWindow="1785" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1413,7 +1413,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,7 +1598,9 @@
       <c r="D9" s="2">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" t="s">

</xml_diff>

<commit_message>
Implement View Inventory Filtering and Stock Remove For Officer Role
Implemented filtering view inventory page and removal of stock items for users with the officer role. Fixed compartment capacity not updating with item removal. Updated tests for compartment and view inventory vm to account for added functionality. Updated README with officer login credentials. Updated sprint backlog remaining task time.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog.xlsx
+++ b/documentation/Sprint Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rs00207\Documents\GitHub\PirateShipInventoryManagementSystem\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DEA193-E697-44BB-823A-8BBE82F51EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46988435-39E2-4867-BC07-F5F94CEC029E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2310" yWindow="1785" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1538,7 +1538,9 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" t="s">
@@ -1558,7 +1560,9 @@
       <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" t="s">
@@ -1578,7 +1582,9 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" t="s">
@@ -1620,7 +1626,9 @@
       <c r="D10" s="2">
         <v>1.5</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" t="s">
@@ -1660,7 +1668,9 @@
       <c r="D12" s="2">
         <v>0</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" t="s">
@@ -1680,7 +1690,9 @@
       <c r="D13" s="2">
         <v>0.5</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" t="s">
@@ -1700,7 +1712,9 @@
       <c r="D14" s="2">
         <v>1</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" t="s">

</xml_diff>

<commit_message>
Implemented Stock History Log for Removal
Implemented inventory history change log for removal of inventory stock items. Updated sprint backlog to update time remaining on tasks.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog.xlsx
+++ b/documentation/Sprint Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rs00207\Documents\GitHub\PirateShipInventoryManagementSystem\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46988435-39E2-4867-BC07-F5F94CEC029E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C035DDDB-7B9B-4434-875A-DD58C355F2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2310" yWindow="1785" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1413,7 +1413,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1648,7 +1648,9 @@
       <c r="D11" s="2">
         <v>0.5</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" t="s">
@@ -1734,7 +1736,9 @@
       <c r="D15" s="2">
         <v>1</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" t="s">

</xml_diff>

<commit_message>
Fix checkstyle errors and Update tests for full coverage
Fixed remaining checkstlye errors, and updated tests to ensure full code coverage within report. Updated readme to include case of non testable code within landingpageviewmodel. Updated sprint backlog for complete implementation.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog.xlsx
+++ b/documentation/Sprint Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rs00207\Documents\GitHub\PirateShipInventoryManagementSystem\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C035DDDB-7B9B-4434-875A-DD58C355F2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DF4F5D-4AB3-4A60-8AC9-6295B8CDE62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2310" yWindow="1785" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -359,13 +359,13 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1412,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,9 +1478,15 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
       <c r="H3" t="s">
         <v>29</v>
       </c>
@@ -1498,9 +1504,15 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
       <c r="H4" t="s">
         <v>29</v>
       </c>
@@ -1516,11 +1528,17 @@
         <v>2</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
       <c r="H5" t="s">
         <v>29</v>
       </c>
@@ -1541,8 +1559,12 @@
       <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
       <c r="H6" t="s">
         <v>27</v>
       </c>
@@ -1563,8 +1585,12 @@
       <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
       <c r="H7" t="s">
         <v>27</v>
       </c>
@@ -1585,8 +1611,12 @@
       <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
       <c r="H8" t="s">
         <v>28</v>
       </c>
@@ -1607,8 +1637,12 @@
       <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
       <c r="H9" t="s">
         <v>28</v>
       </c>
@@ -1629,8 +1663,12 @@
       <c r="E10" s="2">
         <v>0</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
       <c r="H10" t="s">
         <v>28</v>
       </c>
@@ -1649,10 +1687,14 @@
         <v>0.5</v>
       </c>
       <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
       <c r="H11" t="s">
         <v>28</v>
       </c>
@@ -1673,8 +1715,12 @@
       <c r="E12" s="2">
         <v>0</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
       <c r="H12" t="s">
         <v>27</v>
       </c>
@@ -1695,8 +1741,12 @@
       <c r="E13" s="2">
         <v>0</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
       <c r="H13" t="s">
         <v>28</v>
       </c>
@@ -1717,8 +1767,12 @@
       <c r="E14" s="2">
         <v>0</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
       <c r="H14" t="s">
         <v>28</v>
       </c>
@@ -1734,13 +1788,17 @@
         <v>0.5</v>
       </c>
       <c r="D15" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
       <c r="H15" t="s">
         <v>28</v>
       </c>
@@ -1758,9 +1816,15 @@
       <c r="D16" s="2">
         <v>2</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
       <c r="H16" t="s">
         <v>29</v>
       </c>
@@ -1778,9 +1842,15 @@
       <c r="D17" s="2">
         <v>0</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
       <c r="H17" t="s">
         <v>27</v>
       </c>
@@ -1876,15 +1946,15 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" ref="D27:G27" si="0">SUM(D3:D26)</f>
-        <v>10.5</v>
+        <v>11</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="0"/>

</xml_diff>